<commit_message>
static & media files fix
</commit_message>
<xml_diff>
--- a/staticfiles/DocCreation/BFL.xlsx
+++ b/staticfiles/DocCreation/BFL.xlsx
@@ -1085,7 +1085,7 @@
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="57" t="inlineStr">
         <is>
-          <t>Reference Number : 11March2021</t>
+          <t>Reference Number : 17December2020-BFL</t>
         </is>
       </c>
       <c r="B3" s="84" t="n"/>
@@ -1107,7 +1107,7 @@
       <c r="B4" s="86" t="n"/>
       <c r="C4" s="36" t="inlineStr">
         <is>
-          <t>HL</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="D4" s="86" t="n"/>
@@ -1121,7 +1121,7 @@
       <c r="H4" s="85" t="n"/>
       <c r="I4" s="55" t="inlineStr">
         <is>
-          <t>2021-03-11</t>
+          <t>2020-12-17</t>
         </is>
       </c>
       <c r="J4" s="85" t="n"/>
@@ -1141,7 +1141,7 @@
       <c r="H5" s="85" t="n"/>
       <c r="I5" s="36" t="inlineStr">
         <is>
-          <t>John Oliver</t>
+          <t>Morgan</t>
         </is>
       </c>
       <c r="J5" s="85" t="n"/>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="H6" s="85" t="n"/>
       <c r="I6" s="36" t="n">
-        <v>7894561230</v>
+        <v>2267007894</v>
       </c>
       <c r="J6" s="85" t="n"/>
     </row>
@@ -1182,7 +1182,7 @@
       <c r="C7" s="85" t="n"/>
       <c r="D7" s="43" t="inlineStr">
         <is>
-          <t>Mrs. Orca Reddy &amp; Mr. Aryan</t>
+          <t>Mr. &amp; Mrs. Stevansons</t>
         </is>
       </c>
       <c r="E7" s="84" t="n"/>
@@ -1201,7 +1201,7 @@
       <c r="B8" s="85" t="n"/>
       <c r="C8" s="43" t="inlineStr">
         <is>
-          <t>Driver license</t>
+          <t>passport</t>
         </is>
       </c>
       <c r="D8" s="84" t="n"/>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B15" s="36" t="inlineStr">
         <is>
-          <t>78*45*</t>
+          <t>78*15*</t>
         </is>
       </c>
       <c r="C15" s="84" t="n"/>
@@ -1336,7 +1336,7 @@
       <c r="I15" s="85" t="n"/>
       <c r="J15" s="59" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>63</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       <c r="H18" s="85" t="n"/>
       <c r="I18" s="49" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Low</t>
         </is>
       </c>
       <c r="J18" s="85" t="n"/>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="B21" s="43" t="inlineStr">
         <is>
-          <t>Adigas</t>
+          <t>Walmart</t>
         </is>
       </c>
       <c r="C21" s="84" t="n"/>
@@ -1467,7 +1467,7 @@
       <c r="F21" s="85" t="n"/>
       <c r="G21" s="43" t="inlineStr">
         <is>
-          <t>Walmart</t>
+          <t>Adigas</t>
         </is>
       </c>
       <c r="H21" s="84" t="n"/>
@@ -1491,7 +1491,7 @@
       <c r="F22" s="85" t="n"/>
       <c r="G22" s="43" t="inlineStr">
         <is>
-          <t>BigBazar</t>
+          <t>BestBuy</t>
         </is>
       </c>
       <c r="H22" s="84" t="n"/>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="B23" s="44" t="inlineStr">
         <is>
-          <t>WholeFoods</t>
+          <t>PVR</t>
         </is>
       </c>
       <c r="C23" s="84" t="n"/>
@@ -1515,7 +1515,7 @@
       <c r="F23" s="85" t="n"/>
       <c r="G23" s="43" t="inlineStr">
         <is>
-          <t>BMO</t>
+          <t>PVR</t>
         </is>
       </c>
       <c r="H23" s="84" t="n"/>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B24" s="44" t="inlineStr">
         <is>
-          <t>Shopper</t>
+          <t>Shoppers</t>
         </is>
       </c>
       <c r="C24" s="84" t="n"/>
@@ -1539,7 +1539,7 @@
       <c r="F24" s="85" t="n"/>
       <c r="G24" s="43" t="inlineStr">
         <is>
-          <t>Shopper</t>
+          <t>Shoppers</t>
         </is>
       </c>
       <c r="H24" s="84" t="n"/>
@@ -1585,7 +1585,7 @@
       <c r="D26" s="85" t="n"/>
       <c r="E26" s="25" t="inlineStr">
         <is>
-          <t>perfect</t>
+          <t>Perfect</t>
         </is>
       </c>
       <c r="F26" s="84" t="n"/>
@@ -1733,7 +1733,7 @@
       <c r="D33" s="85" t="n"/>
       <c r="E33" s="44" t="inlineStr">
         <is>
-          <t>Commercial</t>
+          <t>Residential</t>
         </is>
       </c>
       <c r="F33" s="84" t="n"/>

</xml_diff>